<commit_message>
Add simple 'MarbleRoller' implementation that randomly drops a marble in the top left corner and then it 'rolls' back and forth to the bottom where it disappears. This will help test whether I can give a good appearance of motion to the marbles. Update Marble Mat.scad so it can be used to generate the STL files for 3D printing Add 19x19 marble plate, back plate, and shadow box STL files Add color fading to ideas to documentation to give marbles a sense of motion Add spreadsheet to verify (column, row) conversion to LED array index function 'XY" Update the XY() function to put the beginning of the LED strip at the bottom right corner instead of the top left corner.
</commit_message>
<xml_diff>
--- a/documentation/Sukh 16mm Marble Sizes.xlsx
+++ b/documentation/Sukh 16mm Marble Sizes.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\MarbleMadness\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86622807-847B-4DE2-887C-9B719D1E7F03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86D3BC0E-D55E-44E1-86F8-91D4380ED03D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51480" yWindow="8490" windowWidth="25440" windowHeight="15270" xr2:uid="{7F599B48-E43F-425B-B627-987D0130B778}"/>
+    <workbookView xWindow="51480" yWindow="8490" windowWidth="25440" windowHeight="15270" activeTab="1" xr2:uid="{7F599B48-E43F-425B-B627-987D0130B778}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Marble Dimensions" sheetId="1" r:id="rId1"/>
+    <sheet name="XY mapping" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>average</t>
   </si>
@@ -51,6 +52,18 @@
   </si>
   <si>
     <t>max</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>base_index</t>
   </si>
 </sst>
 </file>
@@ -435,7 +448,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A312CFE5-D371-448E-A81D-AC0D7DAC7CBD}">
   <dimension ref="B2:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -583,4 +596,1290 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1387A12-1AAF-467E-8C98-7597CE92A201}">
+  <dimension ref="B2:V28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>4</v>
+      </c>
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <v>6</v>
+      </c>
+      <c r="K2">
+        <v>7</v>
+      </c>
+      <c r="L2">
+        <v>8</v>
+      </c>
+      <c r="M2">
+        <v>9</v>
+      </c>
+      <c r="N2">
+        <v>10</v>
+      </c>
+      <c r="O2">
+        <v>11</v>
+      </c>
+      <c r="P2">
+        <v>12</v>
+      </c>
+      <c r="Q2">
+        <v>13</v>
+      </c>
+      <c r="R2">
+        <v>14</v>
+      </c>
+      <c r="S2">
+        <v>15</v>
+      </c>
+      <c r="T2">
+        <v>16</v>
+      </c>
+      <c r="U2">
+        <v>17</v>
+      </c>
+      <c r="V2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>360</v>
+      </c>
+      <c r="E4">
+        <v>359</v>
+      </c>
+      <c r="F4">
+        <v>358</v>
+      </c>
+      <c r="G4">
+        <v>357</v>
+      </c>
+      <c r="H4">
+        <v>356</v>
+      </c>
+      <c r="I4">
+        <v>355</v>
+      </c>
+      <c r="J4">
+        <v>354</v>
+      </c>
+      <c r="K4">
+        <v>353</v>
+      </c>
+      <c r="L4">
+        <v>352</v>
+      </c>
+      <c r="M4">
+        <v>351</v>
+      </c>
+      <c r="N4">
+        <v>350</v>
+      </c>
+      <c r="O4">
+        <v>349</v>
+      </c>
+      <c r="P4">
+        <v>348</v>
+      </c>
+      <c r="Q4">
+        <v>347</v>
+      </c>
+      <c r="R4">
+        <v>346</v>
+      </c>
+      <c r="S4">
+        <v>345</v>
+      </c>
+      <c r="T4">
+        <v>344</v>
+      </c>
+      <c r="U4">
+        <v>343</v>
+      </c>
+      <c r="V4">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>323</v>
+      </c>
+      <c r="E5">
+        <v>324</v>
+      </c>
+      <c r="F5">
+        <v>325</v>
+      </c>
+      <c r="G5">
+        <v>326</v>
+      </c>
+      <c r="H5">
+        <v>327</v>
+      </c>
+      <c r="I5">
+        <v>328</v>
+      </c>
+      <c r="J5">
+        <v>329</v>
+      </c>
+      <c r="K5">
+        <v>330</v>
+      </c>
+      <c r="L5">
+        <v>331</v>
+      </c>
+      <c r="M5">
+        <v>332</v>
+      </c>
+      <c r="N5">
+        <v>333</v>
+      </c>
+      <c r="O5">
+        <v>334</v>
+      </c>
+      <c r="P5">
+        <v>335</v>
+      </c>
+      <c r="Q5">
+        <v>336</v>
+      </c>
+      <c r="R5">
+        <v>337</v>
+      </c>
+      <c r="S5">
+        <v>338</v>
+      </c>
+      <c r="T5">
+        <v>339</v>
+      </c>
+      <c r="U5">
+        <v>340</v>
+      </c>
+      <c r="V5">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>322</v>
+      </c>
+      <c r="E6">
+        <v>321</v>
+      </c>
+      <c r="F6">
+        <v>320</v>
+      </c>
+      <c r="G6">
+        <v>319</v>
+      </c>
+      <c r="H6">
+        <v>318</v>
+      </c>
+      <c r="I6">
+        <v>317</v>
+      </c>
+      <c r="J6">
+        <v>316</v>
+      </c>
+      <c r="K6">
+        <v>315</v>
+      </c>
+      <c r="L6">
+        <v>314</v>
+      </c>
+      <c r="M6">
+        <v>313</v>
+      </c>
+      <c r="N6">
+        <v>312</v>
+      </c>
+      <c r="O6">
+        <v>311</v>
+      </c>
+      <c r="P6">
+        <v>310</v>
+      </c>
+      <c r="Q6">
+        <v>309</v>
+      </c>
+      <c r="R6">
+        <v>308</v>
+      </c>
+      <c r="S6">
+        <v>307</v>
+      </c>
+      <c r="T6">
+        <v>306</v>
+      </c>
+      <c r="U6">
+        <v>305</v>
+      </c>
+      <c r="V6">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>285</v>
+      </c>
+      <c r="E7">
+        <v>286</v>
+      </c>
+      <c r="F7">
+        <v>287</v>
+      </c>
+      <c r="G7">
+        <v>288</v>
+      </c>
+      <c r="H7">
+        <v>289</v>
+      </c>
+      <c r="I7">
+        <v>290</v>
+      </c>
+      <c r="J7">
+        <v>291</v>
+      </c>
+      <c r="K7">
+        <v>292</v>
+      </c>
+      <c r="L7">
+        <v>293</v>
+      </c>
+      <c r="M7">
+        <v>294</v>
+      </c>
+      <c r="N7">
+        <v>295</v>
+      </c>
+      <c r="O7">
+        <v>296</v>
+      </c>
+      <c r="P7">
+        <v>297</v>
+      </c>
+      <c r="Q7">
+        <v>298</v>
+      </c>
+      <c r="R7">
+        <v>299</v>
+      </c>
+      <c r="S7">
+        <v>300</v>
+      </c>
+      <c r="T7">
+        <v>301</v>
+      </c>
+      <c r="U7">
+        <v>302</v>
+      </c>
+      <c r="V7">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>284</v>
+      </c>
+      <c r="E8">
+        <v>283</v>
+      </c>
+      <c r="F8">
+        <v>282</v>
+      </c>
+      <c r="G8">
+        <v>281</v>
+      </c>
+      <c r="H8">
+        <v>280</v>
+      </c>
+      <c r="I8">
+        <v>279</v>
+      </c>
+      <c r="J8">
+        <v>278</v>
+      </c>
+      <c r="K8">
+        <v>277</v>
+      </c>
+      <c r="L8">
+        <v>276</v>
+      </c>
+      <c r="M8">
+        <v>275</v>
+      </c>
+      <c r="N8">
+        <v>274</v>
+      </c>
+      <c r="O8">
+        <v>273</v>
+      </c>
+      <c r="P8">
+        <v>272</v>
+      </c>
+      <c r="Q8">
+        <v>271</v>
+      </c>
+      <c r="R8">
+        <v>270</v>
+      </c>
+      <c r="S8">
+        <v>269</v>
+      </c>
+      <c r="T8">
+        <v>268</v>
+      </c>
+      <c r="U8">
+        <v>267</v>
+      </c>
+      <c r="V8">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>247</v>
+      </c>
+      <c r="E9">
+        <v>248</v>
+      </c>
+      <c r="F9">
+        <v>249</v>
+      </c>
+      <c r="G9">
+        <v>250</v>
+      </c>
+      <c r="H9">
+        <v>251</v>
+      </c>
+      <c r="I9">
+        <v>252</v>
+      </c>
+      <c r="J9">
+        <v>253</v>
+      </c>
+      <c r="K9">
+        <v>254</v>
+      </c>
+      <c r="L9">
+        <v>255</v>
+      </c>
+      <c r="M9">
+        <v>256</v>
+      </c>
+      <c r="N9">
+        <v>257</v>
+      </c>
+      <c r="O9">
+        <v>258</v>
+      </c>
+      <c r="P9">
+        <v>259</v>
+      </c>
+      <c r="Q9">
+        <v>260</v>
+      </c>
+      <c r="R9">
+        <v>261</v>
+      </c>
+      <c r="S9">
+        <v>262</v>
+      </c>
+      <c r="T9">
+        <v>263</v>
+      </c>
+      <c r="U9">
+        <v>264</v>
+      </c>
+      <c r="V9">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <v>246</v>
+      </c>
+      <c r="E10">
+        <v>245</v>
+      </c>
+      <c r="F10">
+        <v>244</v>
+      </c>
+      <c r="G10">
+        <v>243</v>
+      </c>
+      <c r="H10">
+        <v>242</v>
+      </c>
+      <c r="I10">
+        <v>241</v>
+      </c>
+      <c r="J10">
+        <v>240</v>
+      </c>
+      <c r="K10">
+        <v>239</v>
+      </c>
+      <c r="L10">
+        <v>238</v>
+      </c>
+      <c r="M10">
+        <v>237</v>
+      </c>
+      <c r="N10">
+        <v>236</v>
+      </c>
+      <c r="O10">
+        <v>235</v>
+      </c>
+      <c r="P10">
+        <v>234</v>
+      </c>
+      <c r="Q10">
+        <v>233</v>
+      </c>
+      <c r="R10">
+        <v>232</v>
+      </c>
+      <c r="S10">
+        <v>231</v>
+      </c>
+      <c r="T10">
+        <v>230</v>
+      </c>
+      <c r="U10">
+        <v>229</v>
+      </c>
+      <c r="V10">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>7</v>
+      </c>
+      <c r="D11">
+        <v>209</v>
+      </c>
+      <c r="E11">
+        <v>210</v>
+      </c>
+      <c r="F11">
+        <v>211</v>
+      </c>
+      <c r="G11">
+        <v>212</v>
+      </c>
+      <c r="H11">
+        <v>213</v>
+      </c>
+      <c r="I11">
+        <v>214</v>
+      </c>
+      <c r="J11">
+        <v>215</v>
+      </c>
+      <c r="K11">
+        <v>216</v>
+      </c>
+      <c r="L11">
+        <v>217</v>
+      </c>
+      <c r="M11">
+        <v>218</v>
+      </c>
+      <c r="N11">
+        <v>219</v>
+      </c>
+      <c r="O11">
+        <v>220</v>
+      </c>
+      <c r="P11">
+        <v>221</v>
+      </c>
+      <c r="Q11">
+        <v>222</v>
+      </c>
+      <c r="R11">
+        <v>223</v>
+      </c>
+      <c r="S11">
+        <v>224</v>
+      </c>
+      <c r="T11">
+        <v>225</v>
+      </c>
+      <c r="U11">
+        <v>226</v>
+      </c>
+      <c r="V11">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="D12">
+        <v>208</v>
+      </c>
+      <c r="E12">
+        <v>207</v>
+      </c>
+      <c r="F12">
+        <v>206</v>
+      </c>
+      <c r="G12">
+        <v>205</v>
+      </c>
+      <c r="H12">
+        <v>204</v>
+      </c>
+      <c r="I12">
+        <v>203</v>
+      </c>
+      <c r="J12">
+        <v>202</v>
+      </c>
+      <c r="K12">
+        <v>201</v>
+      </c>
+      <c r="L12">
+        <v>200</v>
+      </c>
+      <c r="M12">
+        <v>199</v>
+      </c>
+      <c r="N12">
+        <v>198</v>
+      </c>
+      <c r="O12">
+        <v>197</v>
+      </c>
+      <c r="P12">
+        <v>196</v>
+      </c>
+      <c r="Q12">
+        <v>195</v>
+      </c>
+      <c r="R12">
+        <v>194</v>
+      </c>
+      <c r="S12">
+        <v>193</v>
+      </c>
+      <c r="T12">
+        <v>192</v>
+      </c>
+      <c r="U12">
+        <v>191</v>
+      </c>
+      <c r="V12">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>9</v>
+      </c>
+      <c r="D13">
+        <v>171</v>
+      </c>
+      <c r="E13">
+        <v>172</v>
+      </c>
+      <c r="F13">
+        <v>173</v>
+      </c>
+      <c r="G13">
+        <v>174</v>
+      </c>
+      <c r="H13">
+        <v>175</v>
+      </c>
+      <c r="I13">
+        <v>176</v>
+      </c>
+      <c r="J13">
+        <v>177</v>
+      </c>
+      <c r="K13">
+        <v>178</v>
+      </c>
+      <c r="L13">
+        <v>179</v>
+      </c>
+      <c r="M13">
+        <v>180</v>
+      </c>
+      <c r="N13">
+        <v>181</v>
+      </c>
+      <c r="O13">
+        <v>182</v>
+      </c>
+      <c r="P13">
+        <v>183</v>
+      </c>
+      <c r="Q13">
+        <v>184</v>
+      </c>
+      <c r="R13">
+        <v>185</v>
+      </c>
+      <c r="S13">
+        <v>186</v>
+      </c>
+      <c r="T13">
+        <v>187</v>
+      </c>
+      <c r="U13">
+        <v>188</v>
+      </c>
+      <c r="V13">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>170</v>
+      </c>
+      <c r="E14">
+        <v>169</v>
+      </c>
+      <c r="F14">
+        <v>168</v>
+      </c>
+      <c r="G14">
+        <v>167</v>
+      </c>
+      <c r="H14">
+        <v>166</v>
+      </c>
+      <c r="I14">
+        <v>165</v>
+      </c>
+      <c r="J14">
+        <v>164</v>
+      </c>
+      <c r="K14">
+        <v>163</v>
+      </c>
+      <c r="L14">
+        <v>162</v>
+      </c>
+      <c r="M14">
+        <v>161</v>
+      </c>
+      <c r="N14">
+        <v>160</v>
+      </c>
+      <c r="O14">
+        <v>159</v>
+      </c>
+      <c r="P14">
+        <v>158</v>
+      </c>
+      <c r="Q14">
+        <v>157</v>
+      </c>
+      <c r="R14">
+        <v>156</v>
+      </c>
+      <c r="S14">
+        <v>155</v>
+      </c>
+      <c r="T14">
+        <v>154</v>
+      </c>
+      <c r="U14">
+        <v>153</v>
+      </c>
+      <c r="V14">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>11</v>
+      </c>
+      <c r="D15">
+        <v>133</v>
+      </c>
+      <c r="E15">
+        <v>134</v>
+      </c>
+      <c r="F15">
+        <v>135</v>
+      </c>
+      <c r="G15">
+        <v>136</v>
+      </c>
+      <c r="H15">
+        <v>137</v>
+      </c>
+      <c r="I15">
+        <v>138</v>
+      </c>
+      <c r="J15">
+        <v>139</v>
+      </c>
+      <c r="K15">
+        <v>140</v>
+      </c>
+      <c r="L15">
+        <v>141</v>
+      </c>
+      <c r="M15">
+        <v>142</v>
+      </c>
+      <c r="N15">
+        <v>143</v>
+      </c>
+      <c r="O15">
+        <v>144</v>
+      </c>
+      <c r="P15">
+        <v>145</v>
+      </c>
+      <c r="Q15">
+        <v>146</v>
+      </c>
+      <c r="R15">
+        <v>147</v>
+      </c>
+      <c r="S15">
+        <v>148</v>
+      </c>
+      <c r="T15">
+        <v>149</v>
+      </c>
+      <c r="U15">
+        <v>150</v>
+      </c>
+      <c r="V15">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>12</v>
+      </c>
+      <c r="D16">
+        <v>132</v>
+      </c>
+      <c r="E16">
+        <v>131</v>
+      </c>
+      <c r="F16">
+        <v>130</v>
+      </c>
+      <c r="G16">
+        <v>129</v>
+      </c>
+      <c r="H16">
+        <v>128</v>
+      </c>
+      <c r="I16">
+        <v>127</v>
+      </c>
+      <c r="J16">
+        <v>126</v>
+      </c>
+      <c r="K16">
+        <v>125</v>
+      </c>
+      <c r="L16">
+        <v>124</v>
+      </c>
+      <c r="M16">
+        <v>123</v>
+      </c>
+      <c r="N16">
+        <v>122</v>
+      </c>
+      <c r="O16">
+        <v>121</v>
+      </c>
+      <c r="P16">
+        <v>120</v>
+      </c>
+      <c r="Q16">
+        <v>119</v>
+      </c>
+      <c r="R16">
+        <v>118</v>
+      </c>
+      <c r="S16">
+        <v>117</v>
+      </c>
+      <c r="T16">
+        <v>116</v>
+      </c>
+      <c r="U16">
+        <v>115</v>
+      </c>
+      <c r="V16">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>13</v>
+      </c>
+      <c r="D17">
+        <v>95</v>
+      </c>
+      <c r="E17">
+        <v>96</v>
+      </c>
+      <c r="F17">
+        <v>97</v>
+      </c>
+      <c r="G17">
+        <v>98</v>
+      </c>
+      <c r="H17">
+        <v>99</v>
+      </c>
+      <c r="I17">
+        <v>100</v>
+      </c>
+      <c r="J17">
+        <v>101</v>
+      </c>
+      <c r="K17">
+        <v>102</v>
+      </c>
+      <c r="L17">
+        <v>103</v>
+      </c>
+      <c r="M17">
+        <v>104</v>
+      </c>
+      <c r="N17">
+        <v>105</v>
+      </c>
+      <c r="O17">
+        <v>106</v>
+      </c>
+      <c r="P17">
+        <v>107</v>
+      </c>
+      <c r="Q17">
+        <v>108</v>
+      </c>
+      <c r="R17">
+        <v>109</v>
+      </c>
+      <c r="S17">
+        <v>110</v>
+      </c>
+      <c r="T17">
+        <v>111</v>
+      </c>
+      <c r="U17">
+        <v>112</v>
+      </c>
+      <c r="V17">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>14</v>
+      </c>
+      <c r="D18">
+        <v>94</v>
+      </c>
+      <c r="E18">
+        <v>93</v>
+      </c>
+      <c r="F18">
+        <v>92</v>
+      </c>
+      <c r="G18">
+        <v>91</v>
+      </c>
+      <c r="H18">
+        <v>90</v>
+      </c>
+      <c r="I18">
+        <v>89</v>
+      </c>
+      <c r="J18">
+        <v>88</v>
+      </c>
+      <c r="K18">
+        <v>87</v>
+      </c>
+      <c r="L18">
+        <v>86</v>
+      </c>
+      <c r="M18">
+        <v>85</v>
+      </c>
+      <c r="N18">
+        <v>84</v>
+      </c>
+      <c r="O18">
+        <v>83</v>
+      </c>
+      <c r="P18">
+        <v>82</v>
+      </c>
+      <c r="Q18">
+        <v>81</v>
+      </c>
+      <c r="R18">
+        <v>80</v>
+      </c>
+      <c r="S18">
+        <v>79</v>
+      </c>
+      <c r="T18">
+        <v>78</v>
+      </c>
+      <c r="U18">
+        <v>77</v>
+      </c>
+      <c r="V18">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>15</v>
+      </c>
+      <c r="D19">
+        <v>57</v>
+      </c>
+      <c r="E19">
+        <v>58</v>
+      </c>
+      <c r="F19">
+        <v>59</v>
+      </c>
+      <c r="G19">
+        <v>60</v>
+      </c>
+      <c r="H19">
+        <v>61</v>
+      </c>
+      <c r="I19">
+        <v>62</v>
+      </c>
+      <c r="J19">
+        <v>63</v>
+      </c>
+      <c r="K19">
+        <v>64</v>
+      </c>
+      <c r="L19">
+        <v>65</v>
+      </c>
+      <c r="M19">
+        <v>66</v>
+      </c>
+      <c r="N19">
+        <v>67</v>
+      </c>
+      <c r="O19">
+        <v>68</v>
+      </c>
+      <c r="P19">
+        <v>69</v>
+      </c>
+      <c r="Q19">
+        <v>70</v>
+      </c>
+      <c r="R19">
+        <v>71</v>
+      </c>
+      <c r="S19">
+        <v>72</v>
+      </c>
+      <c r="T19">
+        <v>73</v>
+      </c>
+      <c r="U19">
+        <v>74</v>
+      </c>
+      <c r="V19">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>16</v>
+      </c>
+      <c r="D20">
+        <v>56</v>
+      </c>
+      <c r="E20">
+        <v>55</v>
+      </c>
+      <c r="F20">
+        <v>54</v>
+      </c>
+      <c r="G20">
+        <v>53</v>
+      </c>
+      <c r="H20">
+        <v>52</v>
+      </c>
+      <c r="I20">
+        <v>51</v>
+      </c>
+      <c r="J20">
+        <v>50</v>
+      </c>
+      <c r="K20">
+        <v>49</v>
+      </c>
+      <c r="L20">
+        <v>48</v>
+      </c>
+      <c r="M20">
+        <v>47</v>
+      </c>
+      <c r="N20">
+        <v>46</v>
+      </c>
+      <c r="O20">
+        <v>45</v>
+      </c>
+      <c r="P20">
+        <v>44</v>
+      </c>
+      <c r="Q20">
+        <v>43</v>
+      </c>
+      <c r="R20">
+        <v>42</v>
+      </c>
+      <c r="S20">
+        <v>41</v>
+      </c>
+      <c r="T20">
+        <v>40</v>
+      </c>
+      <c r="U20">
+        <v>39</v>
+      </c>
+      <c r="V20">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>17</v>
+      </c>
+      <c r="D21">
+        <v>19</v>
+      </c>
+      <c r="E21">
+        <v>20</v>
+      </c>
+      <c r="F21">
+        <v>21</v>
+      </c>
+      <c r="G21">
+        <v>22</v>
+      </c>
+      <c r="H21">
+        <v>23</v>
+      </c>
+      <c r="I21">
+        <v>24</v>
+      </c>
+      <c r="J21">
+        <v>25</v>
+      </c>
+      <c r="K21">
+        <v>26</v>
+      </c>
+      <c r="L21">
+        <v>27</v>
+      </c>
+      <c r="M21">
+        <v>28</v>
+      </c>
+      <c r="N21">
+        <v>29</v>
+      </c>
+      <c r="O21">
+        <v>30</v>
+      </c>
+      <c r="P21">
+        <v>31</v>
+      </c>
+      <c r="Q21">
+        <v>32</v>
+      </c>
+      <c r="R21">
+        <v>33</v>
+      </c>
+      <c r="S21">
+        <v>34</v>
+      </c>
+      <c r="T21">
+        <v>35</v>
+      </c>
+      <c r="U21">
+        <v>36</v>
+      </c>
+      <c r="V21">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>18</v>
+      </c>
+      <c r="D22">
+        <v>18</v>
+      </c>
+      <c r="E22">
+        <v>17</v>
+      </c>
+      <c r="F22">
+        <v>16</v>
+      </c>
+      <c r="G22">
+        <v>15</v>
+      </c>
+      <c r="H22">
+        <v>14</v>
+      </c>
+      <c r="I22">
+        <v>13</v>
+      </c>
+      <c r="J22">
+        <v>12</v>
+      </c>
+      <c r="K22">
+        <v>11</v>
+      </c>
+      <c r="L22">
+        <v>10</v>
+      </c>
+      <c r="M22">
+        <v>9</v>
+      </c>
+      <c r="N22">
+        <v>8</v>
+      </c>
+      <c r="O22">
+        <v>7</v>
+      </c>
+      <c r="P22">
+        <v>6</v>
+      </c>
+      <c r="Q22">
+        <v>5</v>
+      </c>
+      <c r="R22">
+        <v>4</v>
+      </c>
+      <c r="S22">
+        <v>3</v>
+      </c>
+      <c r="T22">
+        <v>2</v>
+      </c>
+      <c r="U22">
+        <v>1</v>
+      </c>
+      <c r="V22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <f>IF(ISEVEN(C26), C26*19+C25, C26*19+(19-1-C25))</f>
+        <v>359</v>
+      </c>
+    </row>
+    <row r="28" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28">
+        <f>(19*19-1)-C27</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>